<commit_message>
calculo de estatísticas de erro parcial
</commit_message>
<xml_diff>
--- a/models/dissertation-model/modelo-R/calibracao/dados_calibracao.xlsx
+++ b/models/dissertation-model/modelo-R/calibracao/dados_calibracao.xlsx
@@ -433,14 +433,12 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.3061224489796"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -453,7 +451,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>0</v>
+        <v>2007</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>2600</v>
@@ -462,7 +460,7 @@
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <f aca="false">A2+1</f>
-        <v>1</v>
+        <v>2008</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>3500</v>
@@ -471,7 +469,7 @@
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <f aca="false">A3+1</f>
-        <v>2</v>
+        <v>2009</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>4000</v>
@@ -480,7 +478,7 @@
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <f aca="false">A4+1</f>
-        <v>3</v>
+        <v>2010</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>5000</v>
@@ -489,7 +487,7 @@
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <f aca="false">A5+1</f>
-        <v>4</v>
+        <v>2011</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>5050</v>
@@ -498,7 +496,7 @@
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <f aca="false">A6+1</f>
-        <v>5</v>
+        <v>2012</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>4600</v>
@@ -507,7 +505,7 @@
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <f aca="false">A7+1</f>
-        <v>6</v>
+        <v>2013</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>6100</v>
@@ -516,7 +514,7 @@
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <f aca="false">A8+1</f>
-        <v>7</v>
+        <v>2014</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>6500</v>
@@ -525,7 +523,7 @@
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <f aca="false">A9+1</f>
-        <v>8</v>
+        <v>2015</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>7771</v>
@@ -534,7 +532,7 @@
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <f aca="false">A10+1</f>
-        <v>9</v>
+        <v>2016</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>10310.5</v>
@@ -543,7 +541,7 @@
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <f aca="false">A11+1</f>
-        <v>10</v>
+        <v>2017</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>12850</v>
@@ -573,12 +571,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.4438775510204"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.9387755102041"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.1326530612245"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.530612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.7295918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -694,13 +692,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="10" min="2" style="1" width="39.5510204081633"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="43.0612244897959"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="42.6581632653061"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="38.6071428571429"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="40.6326530612245"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="10" min="2" style="1" width="39.1479591836735"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="42.5204081632653"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="42.25"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="38.0663265306122"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="40.0918367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1664,8 +1662,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.5867346938776"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.1836734693878"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1827,9 +1825,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1931,7 +1929,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Adicionando material para calibrar o modelo
</commit_message>
<xml_diff>
--- a/models/dissertation-model/modelo-R/calibracao/dados_calibracao.xlsx
+++ b/models/dissertation-model/modelo-R/calibracao/dados_calibracao.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="69">
   <si>
     <t xml:space="preserve">time</t>
   </si>
@@ -141,6 +141,9 @@
     <t xml:space="preserve">Margem Média - Fornecedores de Materiais de Impressão</t>
   </si>
   <si>
+    <t xml:space="preserve">Média</t>
+  </si>
+  <si>
     <t xml:space="preserve">Market Share 3D System Manufacturers</t>
   </si>
   <si>
@@ -198,9 +201,15 @@
     <t xml:space="preserve">Patentes Publicadas</t>
   </si>
   <si>
+    <t xml:space="preserve">Share</t>
+  </si>
+  <si>
     <t xml:space="preserve">Fujitsu</t>
   </si>
   <si>
+    <t xml:space="preserve">x</t>
+  </si>
+  <si>
     <t xml:space="preserve">NEC Corp</t>
   </si>
   <si>
@@ -214,6 +223,9 @@
   </si>
   <si>
     <t xml:space="preserve">Univ Texas System</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total</t>
   </si>
   <si>
     <t xml:space="preserve">2015: Systems Manufacturers 55% do Mercado Total, Service Providers 25%</t>
@@ -315,7 +327,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -349,6 +361,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -432,13 +448,15 @@
   </sheetPr>
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -571,12 +589,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.530612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.7295918367347"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.1275510204082"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.3214285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -680,25 +698,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N35"/>
+  <dimension ref="A1:O36"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="C27" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="L28" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
-      <selection pane="bottomRight" activeCell="D22" activeCellId="0" sqref="D22"/>
+      <selection pane="topRight" activeCell="L1" activeCellId="0" sqref="L1"/>
+      <selection pane="bottomLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
+      <selection pane="bottomRight" activeCell="O36" activeCellId="0" sqref="O36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="10" min="2" style="1" width="39.1479591836735"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="42.5204081632653"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="42.25"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="38.0663265306122"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="40.0918367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="10" min="2" style="1" width="38.6071428571429"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="42.1173469387755"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="41.7142857142857"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="37.5255102040816"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="39.6887755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1399,7 +1417,7 @@
         <v>0.172</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
         <v>2010</v>
       </c>
@@ -1430,8 +1448,11 @@
       <c r="K28" s="6" t="n">
         <v>0.196</v>
       </c>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O28" s="0" t="n">
+        <v>10725000</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
         <v>2011</v>
       </c>
@@ -1471,8 +1492,11 @@
       <c r="N29" s="7" t="n">
         <v>0.14</v>
       </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O29" s="0" t="n">
+        <v>14331000</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
         <v>2012</v>
       </c>
@@ -1512,8 +1536,11 @@
       <c r="N30" s="7" t="n">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O30" s="0" t="n">
+        <v>23203000</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
         <v>2013</v>
       </c>
@@ -1545,8 +1572,11 @@
       <c r="N31" s="7" t="n">
         <v>0.16</v>
       </c>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O31" s="0" t="n">
+        <v>43489000</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
         <v>2014</v>
       </c>
@@ -1575,8 +1605,11 @@
       <c r="N32" s="7" t="n">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O32" s="0" t="n">
+        <v>75395000</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
         <v>2015</v>
       </c>
@@ -1599,8 +1632,11 @@
       <c r="N33" s="7" t="n">
         <v>0.14</v>
       </c>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O33" s="0" t="n">
+        <v>92770000</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
         <v>2016</v>
       </c>
@@ -1614,6 +1650,9 @@
       <c r="J34" s="5" t="n">
         <v>0.55</v>
       </c>
+      <c r="O34" s="0" t="n">
+        <v>88395000</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
@@ -1625,6 +1664,63 @@
       </c>
       <c r="J35" s="5" t="n">
         <v>0.55</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36" s="1" t="n">
+        <f aca="false">AVERAGE(B6:B35)</f>
+        <v>241.294117647059</v>
+      </c>
+      <c r="C36" s="1" t="n">
+        <f aca="false">AVERAGE(C6:C35)</f>
+        <v>35009.375</v>
+      </c>
+      <c r="D36" s="1" t="n">
+        <f aca="false">AVERAGE(D6:D35)</f>
+        <v>2934.42592592593</v>
+      </c>
+      <c r="E36" s="1" t="e">
+        <f aca="false">AVERAGE(E6:E35)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F36" s="1" t="e">
+        <f aca="false">AVERAGE(F6:F35)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G36" s="1" t="n">
+        <f aca="false">AVERAGE(G6:G35)</f>
+        <v>185.615384615385</v>
+      </c>
+      <c r="H36" s="1" t="n">
+        <f aca="false">AVERAGE(H6:H35)</f>
+        <v>354.307692307692</v>
+      </c>
+      <c r="I36" s="1" t="n">
+        <f aca="false">AVERAGE(I6:I35)</f>
+        <v>2.27770859277709</v>
+      </c>
+      <c r="J36" s="9" t="n">
+        <f aca="false">AVERAGE(J6:J35)</f>
+        <v>0.55</v>
+      </c>
+      <c r="K36" s="9" t="n">
+        <f aca="false">AVERAGE(K6:K35)</f>
+        <v>0.1432</v>
+      </c>
+      <c r="L36" s="9" t="n">
+        <f aca="false">AVERAGE(L6:L35)</f>
+        <v>0.108</v>
+      </c>
+      <c r="M36" s="9" t="n">
+        <f aca="false">AVERAGE(M6:M35)</f>
+        <v>0.2</v>
+      </c>
+      <c r="N36" s="9" t="n">
+        <f aca="false">AVERAGE(N6:N35)</f>
+        <v>0.148</v>
       </c>
     </row>
   </sheetData>
@@ -1657,13 +1753,13 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.1836734693878"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1673,12 +1769,12 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B3" s="7" t="n">
         <v>0.29</v>
@@ -1686,7 +1782,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B4" s="7" t="n">
         <v>0.28</v>
@@ -1694,7 +1790,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B5" s="7" t="n">
         <v>0.12</v>
@@ -1702,7 +1798,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B6" s="7" t="n">
         <v>0.03</v>
@@ -1710,7 +1806,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B7" s="7" t="n">
         <v>0.03</v>
@@ -1718,7 +1814,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B8" s="7" t="n">
         <v>0.02</v>
@@ -1726,7 +1822,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B9" s="7" t="n">
         <v>0.03</v>
@@ -1734,7 +1830,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B10" s="7" t="n">
         <v>0.03</v>
@@ -1742,7 +1838,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B11" s="7" t="n">
         <v>0.17</v>
@@ -1750,12 +1846,12 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B15" s="7" t="n">
         <v>0.55</v>
@@ -1763,7 +1859,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B16" s="7" t="n">
         <v>0.13</v>
@@ -1771,7 +1867,7 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B17" s="7" t="n">
         <v>0.05</v>
@@ -1779,7 +1875,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B18" s="7" t="n">
         <v>0.02</v>
@@ -1787,7 +1883,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B19" s="7" t="n">
         <v>0.01</v>
@@ -1795,7 +1891,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B20" s="7" t="n">
         <v>0.24</v>
@@ -1817,25 +1913,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>58</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>25</v>
@@ -1843,66 +1942,128 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>92</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C2" s="0" t="n">
+        <f aca="false">B2/$B$10</f>
+        <v>0.182178217821782</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>92</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C3" s="0" t="n">
+        <f aca="false">B3/$B$10</f>
+        <v>0.182178217821782</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <f aca="false">SUM(B2:B3)</f>
+        <v>184</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>91</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C4" s="0" t="n">
+        <f aca="false">B4/$B$10</f>
+        <v>0.18019801980198</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>67</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C5" s="0" t="n">
+        <f aca="false">B5/$B$10</f>
+        <v>0.132673267326733</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <f aca="false">D3/E3</f>
+        <v>306.666666666667</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>48</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="0" t="n">
+        <f aca="false">B6/$B$10</f>
+        <v>0.095049504950495</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>41</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C7" s="0" t="n">
+        <f aca="false">B7/$B$10</f>
+        <v>0.0811881188118812</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>38</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C8" s="0" t="n">
+        <f aca="false">B8/$B$10</f>
+        <v>0.0752475247524752</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>36</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <f aca="false">B9/$B$10</f>
+        <v>0.0712871287128713</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <f aca="false">SUM(B2:B9)</f>
+        <v>505</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <f aca="false">B10/$B$10</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1929,17 +2090,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
solução temp para calibração de condições iniciais
investigar melhor modelagem da calibração dos valores inicias de cumultative adopters
</commit_message>
<xml_diff>
--- a/models/dissertation-model/modelo-R/calibracao/dados_calibracao.xlsx
+++ b/models/dissertation-model/modelo-R/calibracao/dados_calibracao.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" state="visible" r:id="rId2"/>
@@ -30,7 +30,7 @@
     <t xml:space="preserve">time</t>
   </si>
   <si>
-    <t xml:space="preserve">fIndustryOrderRate</t>
+    <t xml:space="preserve">aIndustryShipments</t>
   </si>
   <si>
     <t xml:space="preserve">ReferencePopulation</t>
@@ -448,15 +448,15 @@
   </sheetPr>
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -589,12 +589,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.9030612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.1275510204082"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.3214285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.7244897959184"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.9183673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -710,13 +710,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="10" min="2" style="1" width="38.6071428571429"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="42.1173469387755"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="41.7142857142857"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="37.5255102040816"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="39.6887755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="10" min="2" style="1" width="38.0663265306122"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="41.5765306122449"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="41.1734693877551"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="37.1224489795918"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="39.280612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1556,6 +1556,8 @@
       </c>
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
+      <c r="G31" s="0"/>
+      <c r="H31" s="0"/>
       <c r="I31" s="1" t="n">
         <f aca="false">9145/4015</f>
         <v>2.27770859277709</v>
@@ -1589,6 +1591,10 @@
       <c r="D32" s="1" t="n">
         <v>12850</v>
       </c>
+      <c r="E32" s="0"/>
+      <c r="F32" s="0"/>
+      <c r="G32" s="0"/>
+      <c r="H32" s="0"/>
       <c r="I32" s="1" t="n">
         <f aca="false">9145/4015</f>
         <v>2.27770859277709</v>
@@ -1616,6 +1622,12 @@
       <c r="B33" s="1" t="n">
         <v>850</v>
       </c>
+      <c r="C33" s="0"/>
+      <c r="D33" s="0"/>
+      <c r="E33" s="0"/>
+      <c r="F33" s="0"/>
+      <c r="G33" s="0"/>
+      <c r="H33" s="0"/>
       <c r="I33" s="1" t="n">
         <f aca="false">9145/4015</f>
         <v>2.27770859277709</v>
@@ -1643,6 +1655,12 @@
       <c r="B34" s="1" t="n">
         <v>957</v>
       </c>
+      <c r="C34" s="0"/>
+      <c r="D34" s="0"/>
+      <c r="E34" s="0"/>
+      <c r="F34" s="0"/>
+      <c r="G34" s="0"/>
+      <c r="H34" s="0"/>
       <c r="I34" s="1" t="n">
         <f aca="false">9145/4015</f>
         <v>2.27770859277709</v>
@@ -1658,6 +1676,13 @@
       <c r="A35" s="0" t="n">
         <v>2017</v>
       </c>
+      <c r="B35" s="0"/>
+      <c r="C35" s="0"/>
+      <c r="D35" s="0"/>
+      <c r="E35" s="0"/>
+      <c r="F35" s="0"/>
+      <c r="G35" s="0"/>
+      <c r="H35" s="0"/>
       <c r="I35" s="1" t="n">
         <f aca="false">9145/4015</f>
         <v>2.27770859277709</v>
@@ -1758,8 +1783,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.780612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.3724489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1915,15 +1940,15 @@
   </sheetPr>
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2090,7 +2115,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
gráfico de dispersão por lever
</commit_message>
<xml_diff>
--- a/models/dissertation-model/modelo-R/calibracao/dados_calibracao.xlsx
+++ b/models/dissertation-model/modelo-R/calibracao/dados_calibracao.xlsx
@@ -124,9 +124,6 @@
     <t>http://wohlersassociates.com/blog/2016/01/popularity-of-fdm/</t>
   </si>
   <si>
-    <t>Período dede 88: http://docplayer.net/9034750-Executive-summary-wohlers-report-rapid-prototyping-tooling-state-of-the-industry-annual-worldwide-progress-report.html</t>
-  </si>
-  <si>
     <t>http://www.ey.com/Publication/vwLUAssets/ey-global-3d-printing-report-2016-full-report/$FILE/ey-global-3d-printing-report-2016-full-report.pdf</t>
   </si>
   <si>
@@ -236,6 +233,10 @@
   </si>
   <si>
     <t>3DP Services - aroximadamente 20 a 30% da receita dos Manufacturers</t>
+  </si>
+  <si>
+    <t>Período dede 88: http://docplayer.net/9034750-Executive-summary-wohlers-report-rapid-prototyping-tooling-state-of-the-industry-annual-worldwide-progress-report.html
+Venda em 2014: obtida em https://wohlersassociates.com/blog/2016/01/popularity-of-fdm/</t>
   </si>
 </sst>
 </file>
@@ -933,10 +934,10 @@
   <dimension ref="A1:O36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="B27" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="B31" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="A28" sqref="A28"/>
-      <selection pane="bottomRight" activeCell="D32" sqref="D32"/>
+      <selection pane="bottomRight" activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1044,7 +1045,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>29</v>
       </c>
@@ -1052,7 +1053,7 @@
         <v>30</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>31</v>
+        <v>68</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -1064,18 +1065,18 @@
         <v>24</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5"/>
       <c r="D5"/>
@@ -1086,16 +1087,16 @@
       <c r="I5"/>
       <c r="J5"/>
       <c r="K5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="M5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="N5" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -1924,7 +1925,7 @@
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B36" s="1">
         <f t="shared" ref="B36:N36" si="2">AVERAGE(B6:B35)</f>
@@ -2012,17 +2013,17 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3" s="7">
         <v>0.28999999999999998</v>
@@ -2030,7 +2031,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B4" s="7">
         <v>0.28000000000000003</v>
@@ -2038,7 +2039,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5" s="7">
         <v>0.12</v>
@@ -2046,7 +2047,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B6" s="7">
         <v>0.03</v>
@@ -2054,7 +2055,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B7" s="7">
         <v>0.03</v>
@@ -2062,7 +2063,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B8" s="7">
         <v>0.02</v>
@@ -2070,7 +2071,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B9" s="7">
         <v>0.03</v>
@@ -2078,7 +2079,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B10" s="7">
         <v>0.03</v>
@@ -2086,7 +2087,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B11" s="7">
         <v>0.17</v>
@@ -2094,12 +2095,12 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B15" s="7">
         <v>0.55000000000000004</v>
@@ -2107,7 +2108,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B16" s="7">
         <v>0.13</v>
@@ -2115,7 +2116,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B17" s="7">
         <v>0.05</v>
@@ -2123,7 +2124,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B18" s="7">
         <v>0.02</v>
@@ -2131,7 +2132,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B19" s="7">
         <v>0.01</v>
@@ -2139,7 +2140,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B20" s="7">
         <v>0.24</v>
@@ -2168,13 +2169,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" t="s">
         <v>56</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>57</v>
-      </c>
-      <c r="C1" t="s">
-        <v>58</v>
       </c>
       <c r="D1" t="s">
         <v>25</v>
@@ -2182,7 +2183,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2">
         <v>92</v>
@@ -2194,7 +2195,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3">
         <v>92</v>
@@ -2213,7 +2214,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B4">
         <v>91</v>
@@ -2223,7 +2224,7 @@
         <v>0.18019801980198019</v>
       </c>
       <c r="D4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -2231,7 +2232,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B5">
         <v>67</v>
@@ -2247,7 +2248,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B6">
         <v>48</v>
@@ -2259,7 +2260,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B7">
         <v>41</v>
@@ -2271,7 +2272,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B8">
         <v>38</v>
@@ -2283,7 +2284,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B9">
         <v>36</v>
@@ -2295,7 +2296,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B10">
         <f>SUM(B2:B9)</f>
@@ -2327,12 +2328,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>